<commit_message>
finished functionality of extracting coefficients (choosing begin/end index).
</commit_message>
<xml_diff>
--- a/oneau-loader/src/test/doc/ascp2000-analysis.xlsx
+++ b/oneau-loader/src/test/doc/ascp2000-analysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="1076">
   <si>
     <t>0.245153650000000000D+07</t>
   </si>
@@ -3099,9 +3099,6 @@
     <t>x2</t>
   </si>
   <si>
-    <t xml:space="preserve">sub interval </t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -3214,13 +3211,49 @@
   </si>
   <si>
     <t>POFFSET(IDX)</t>
+  </si>
+  <si>
+    <t>ptr</t>
+  </si>
+  <si>
+    <t>coeff intv</t>
+  </si>
+  <si>
+    <t>venus</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>z2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>z3</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>y4</t>
+  </si>
+  <si>
+    <t>z4</t>
+  </si>
+  <si>
+    <t>idx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3252,6 +3285,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3279,7 +3319,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3299,8 +3339,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3318,8 +3390,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3329,6 +3402,22 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3338,6 +3427,22 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3669,8 +3774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A82" sqref="A81:XFD82"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172:J201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3694,8 +3799,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
+      <c r="A1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1075</v>
+      </c>
       <c r="I1" s="1" t="s">
-        <v>1026</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -3712,13 +3823,13 @@
         <v>1019</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="S2">
         <v>2455439.5</v>
       </c>
       <c r="T2" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -3735,13 +3846,13 @@
         <v>1020</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="S3">
         <v>2305424.5</v>
       </c>
       <c r="T3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -3785,13 +3896,13 @@
         <v>31</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="S4">
         <v>32</v>
       </c>
       <c r="T4" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -3835,7 +3946,7 @@
         <v>32</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="S5" s="6">
         <f>(S2-S3)/S4</f>
@@ -3883,14 +3994,14 @@
         <v>33</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="S6">
         <f>FLOOR(S5, 1)</f>
         <v>4687</v>
       </c>
       <c r="T6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -4016,25 +4127,25 @@
         <v>36</v>
       </c>
       <c r="S9" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="T9" s="2" t="s">
         <v>1036</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="U9" s="2" t="s">
         <v>1037</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>1038</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="W9" s="2" t="s">
         <v>1039</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>1040</v>
       </c>
-      <c r="X9" s="2" t="s">
+      <c r="Y9" s="2" t="s">
         <v>1041</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -4078,7 +4189,7 @@
         <v>37</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="S10" s="3">
         <v>1</v>
@@ -4096,10 +4207,10 @@
         <v>1</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -4143,7 +4254,7 @@
         <v>38</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="S11" s="3">
         <v>2</v>
@@ -4161,10 +4272,10 @@
         <v>1</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -4208,7 +4319,7 @@
         <v>39</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="S12" s="3">
         <v>3</v>
@@ -4273,7 +4384,7 @@
         <v>40</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="S13" s="3">
         <v>171</v>
@@ -4338,7 +4449,7 @@
         <v>41</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="S14" s="3">
         <v>231</v>
@@ -4403,7 +4514,7 @@
         <v>42</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="S15" s="3">
         <v>309</v>
@@ -4468,7 +4579,7 @@
         <v>43</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="S16" s="3">
         <v>342</v>
@@ -4533,7 +4644,7 @@
         <v>44</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="S17" s="3">
         <v>366</v>
@@ -4589,7 +4700,7 @@
         <v>1023</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="S18" s="3">
         <v>387</v>
@@ -4645,7 +4756,7 @@
         <v>1023</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="S19" s="3">
         <v>405</v>
@@ -4701,7 +4812,7 @@
         <v>1023</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="S20" s="3">
         <v>423</v>
@@ -4757,7 +4868,7 @@
         <v>1023</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="S21" s="3">
         <v>441</v>
@@ -4813,7 +4924,7 @@
         <v>1023</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="S22" s="3">
         <v>753</v>
@@ -4869,7 +4980,7 @@
         <v>1023</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="S23" s="3">
         <v>819</v>
@@ -4925,7 +5036,7 @@
         <v>1023</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="S24" s="3">
         <v>899</v>
@@ -5112,7 +5223,7 @@
         <v>1023</v>
       </c>
       <c r="R29" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="S29">
         <v>2451544.5</v>
@@ -5150,7 +5261,7 @@
         <v>1023</v>
       </c>
       <c r="R30" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="S30">
         <v>2451536.5</v>
@@ -5188,7 +5299,7 @@
         <v>1023</v>
       </c>
       <c r="R31" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="S31">
         <v>32</v>
@@ -5226,7 +5337,7 @@
         <v>1024</v>
       </c>
       <c r="R32" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="S32">
         <f>(S29-S30)/S31</f>
@@ -5265,7 +5376,7 @@
         <v>1024</v>
       </c>
       <c r="R33" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="S33">
         <f>FLOOR(S32,1)</f>
@@ -5304,7 +5415,7 @@
         <v>1024</v>
       </c>
       <c r="R34" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="S34">
         <f>(S32-S33)*U12</f>
@@ -5343,7 +5454,7 @@
         <v>1024</v>
       </c>
       <c r="R35" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="S35">
         <f>FLOOR(S34,1)</f>
@@ -5382,7 +5493,7 @@
         <v>1024</v>
       </c>
       <c r="R36" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="S36">
         <f>2*(S34-S35)-1</f>
@@ -5421,7 +5532,7 @@
         <v>1024</v>
       </c>
       <c r="R37" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="S37">
         <f>S12+S35*T12*V12-1</f>
@@ -5460,7 +5571,7 @@
         <v>1024</v>
       </c>
       <c r="R38" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="S38">
         <f>S37+T12*V12-1</f>
@@ -5499,7 +5610,7 @@
         <v>1024</v>
       </c>
       <c r="R39" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="S39">
         <f>S37-2</f>
@@ -5538,7 +5649,7 @@
         <v>1024</v>
       </c>
       <c r="R40" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="41" spans="1:19">
@@ -6304,7 +6415,7 @@
         <v>2</v>
       </c>
       <c r="J60" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -6336,7 +6447,7 @@
         <v>2</v>
       </c>
       <c r="J61" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -6368,7 +6479,7 @@
         <v>2</v>
       </c>
       <c r="J62" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -6400,7 +6511,7 @@
         <v>2</v>
       </c>
       <c r="J63" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -6432,7 +6543,7 @@
         <v>2</v>
       </c>
       <c r="J64" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -6464,7 +6575,7 @@
         <v>2</v>
       </c>
       <c r="J65" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -6496,7 +6607,7 @@
         <v>2</v>
       </c>
       <c r="J66" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -6528,7 +6639,7 @@
         <v>2</v>
       </c>
       <c r="J67" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -6560,7 +6671,7 @@
         <v>2</v>
       </c>
       <c r="J68" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -6592,7 +6703,7 @@
         <v>2</v>
       </c>
       <c r="J69" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -6624,7 +6735,7 @@
         <v>2</v>
       </c>
       <c r="J70" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -6656,7 +6767,7 @@
         <v>2</v>
       </c>
       <c r="J71" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -6688,7 +6799,7 @@
         <v>2</v>
       </c>
       <c r="J72" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -6720,7 +6831,7 @@
         <v>2</v>
       </c>
       <c r="J73" t="s">
-        <v>1023</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -6752,7 +6863,7 @@
         <v>2</v>
       </c>
       <c r="J74" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -6784,7 +6895,7 @@
         <v>2</v>
       </c>
       <c r="J75" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -6816,7 +6927,7 @@
         <v>2</v>
       </c>
       <c r="J76" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -6848,7 +6959,7 @@
         <v>2</v>
       </c>
       <c r="J77" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -6880,7 +6991,7 @@
         <v>2</v>
       </c>
       <c r="J78" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -6912,7 +7023,7 @@
         <v>2</v>
       </c>
       <c r="J79" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -6944,7 +7055,7 @@
         <v>2</v>
       </c>
       <c r="J80" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -6976,7 +7087,7 @@
         <v>2</v>
       </c>
       <c r="J81" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -7008,7 +7119,7 @@
         <v>2</v>
       </c>
       <c r="J82" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="83" spans="1:13">
@@ -7040,7 +7151,7 @@
         <v>2</v>
       </c>
       <c r="J83" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="84" spans="1:13">
@@ -7072,7 +7183,7 @@
         <v>2</v>
       </c>
       <c r="J84" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="85" spans="1:13">
@@ -7104,7 +7215,7 @@
         <v>2</v>
       </c>
       <c r="J85" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -7136,7 +7247,7 @@
         <v>2</v>
       </c>
       <c r="J86" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="87" spans="1:13">
@@ -7168,7 +7279,7 @@
         <v>2</v>
       </c>
       <c r="J87" t="s">
-        <v>1024</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="88" spans="1:13">
@@ -7200,7 +7311,7 @@
         <v>3</v>
       </c>
       <c r="J88" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K88">
         <v>87</v>
@@ -7241,7 +7352,7 @@
         <v>3</v>
       </c>
       <c r="J89" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K89">
         <v>88</v>
@@ -7282,7 +7393,7 @@
         <v>3</v>
       </c>
       <c r="J90" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K90">
         <v>89</v>
@@ -7323,7 +7434,7 @@
         <v>3</v>
       </c>
       <c r="J91" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K91">
         <v>90</v>
@@ -7364,7 +7475,7 @@
         <v>3</v>
       </c>
       <c r="J92" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K92">
         <v>91</v>
@@ -7405,7 +7516,7 @@
         <v>3</v>
       </c>
       <c r="J93" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K93">
         <v>92</v>
@@ -7446,7 +7557,7 @@
         <v>3</v>
       </c>
       <c r="J94" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K94">
         <v>93</v>
@@ -7487,7 +7598,7 @@
         <v>3</v>
       </c>
       <c r="J95" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K95">
         <v>94</v>
@@ -7528,7 +7639,7 @@
         <v>3</v>
       </c>
       <c r="J96" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K96">
         <v>95</v>
@@ -7569,7 +7680,7 @@
         <v>3</v>
       </c>
       <c r="J97" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K97">
         <v>96</v>
@@ -7610,7 +7721,7 @@
         <v>3</v>
       </c>
       <c r="J98" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K98">
         <v>97</v>
@@ -7651,7 +7762,7 @@
         <v>3</v>
       </c>
       <c r="J99" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K99">
         <v>98</v>
@@ -7692,7 +7803,7 @@
         <v>3</v>
       </c>
       <c r="J100" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K100">
         <v>99</v>
@@ -7733,7 +7844,7 @@
         <v>3</v>
       </c>
       <c r="J101" t="s">
-        <v>1022</v>
+        <v>1069</v>
       </c>
       <c r="K101">
         <v>100</v>
@@ -7774,7 +7885,7 @@
         <v>3</v>
       </c>
       <c r="J102" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="103" spans="1:13">
@@ -7806,7 +7917,7 @@
         <v>3</v>
       </c>
       <c r="J103" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -7838,7 +7949,7 @@
         <v>3</v>
       </c>
       <c r="J104" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="105" spans="1:13">
@@ -7870,7 +7981,7 @@
         <v>3</v>
       </c>
       <c r="J105" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="106" spans="1:13">
@@ -7902,7 +8013,7 @@
         <v>3</v>
       </c>
       <c r="J106" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="107" spans="1:13">
@@ -7934,7 +8045,7 @@
         <v>3</v>
       </c>
       <c r="J107" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="108" spans="1:13">
@@ -7966,7 +8077,7 @@
         <v>3</v>
       </c>
       <c r="J108" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="109" spans="1:13">
@@ -7998,7 +8109,7 @@
         <v>3</v>
       </c>
       <c r="J109" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="110" spans="1:13">
@@ -8030,7 +8141,7 @@
         <v>3</v>
       </c>
       <c r="J110" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="111" spans="1:13">
@@ -8062,7 +8173,7 @@
         <v>3</v>
       </c>
       <c r="J111" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="112" spans="1:13">
@@ -8094,7 +8205,7 @@
         <v>3</v>
       </c>
       <c r="J112" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -8126,7 +8237,7 @@
         <v>3</v>
       </c>
       <c r="J113" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -8158,7 +8269,7 @@
         <v>3</v>
       </c>
       <c r="J114" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="115" spans="1:10">
@@ -8190,7 +8301,7 @@
         <v>3</v>
       </c>
       <c r="J115" t="s">
-        <v>1023</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="116" spans="1:10">
@@ -8222,7 +8333,7 @@
         <v>3</v>
       </c>
       <c r="J116" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -8254,7 +8365,7 @@
         <v>3</v>
       </c>
       <c r="J117" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="118" spans="1:10">
@@ -8286,7 +8397,7 @@
         <v>3</v>
       </c>
       <c r="J118" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="119" spans="1:10">
@@ -8318,7 +8429,7 @@
         <v>3</v>
       </c>
       <c r="J119" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="120" spans="1:10">
@@ -8350,7 +8461,7 @@
         <v>3</v>
       </c>
       <c r="J120" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="121" spans="1:10">
@@ -8382,7 +8493,7 @@
         <v>3</v>
       </c>
       <c r="J121" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="122" spans="1:10">
@@ -8414,7 +8525,7 @@
         <v>3</v>
       </c>
       <c r="J122" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="123" spans="1:10">
@@ -8446,7 +8557,7 @@
         <v>3</v>
       </c>
       <c r="J123" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="124" spans="1:10">
@@ -8478,7 +8589,7 @@
         <v>3</v>
       </c>
       <c r="J124" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -8510,7 +8621,7 @@
         <v>3</v>
       </c>
       <c r="J125" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="126" spans="1:10">
@@ -8542,7 +8653,7 @@
         <v>3</v>
       </c>
       <c r="J126" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="127" spans="1:10">
@@ -8574,7 +8685,7 @@
         <v>3</v>
       </c>
       <c r="J127" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="128" spans="1:10">
@@ -8606,7 +8717,7 @@
         <v>3</v>
       </c>
       <c r="J128" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="129" spans="1:13">
@@ -8638,7 +8749,7 @@
         <v>3</v>
       </c>
       <c r="J129" t="s">
-        <v>1024</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="130" spans="1:13">
@@ -8670,7 +8781,7 @@
         <v>4</v>
       </c>
       <c r="J130" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K130">
         <v>129</v>
@@ -8711,7 +8822,7 @@
         <v>4</v>
       </c>
       <c r="J131" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K131">
         <v>130</v>
@@ -8752,7 +8863,7 @@
         <v>4</v>
       </c>
       <c r="J132" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K132">
         <v>131</v>
@@ -8793,7 +8904,7 @@
         <v>4</v>
       </c>
       <c r="J133" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K133">
         <v>132</v>
@@ -8834,7 +8945,7 @@
         <v>4</v>
       </c>
       <c r="J134" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K134">
         <v>133</v>
@@ -8875,7 +8986,7 @@
         <v>4</v>
       </c>
       <c r="J135" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K135">
         <v>134</v>
@@ -8916,7 +9027,7 @@
         <v>4</v>
       </c>
       <c r="J136" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K136">
         <v>135</v>
@@ -8957,7 +9068,7 @@
         <v>4</v>
       </c>
       <c r="J137" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K137">
         <v>136</v>
@@ -8998,7 +9109,7 @@
         <v>4</v>
       </c>
       <c r="J138" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K138">
         <v>137</v>
@@ -9039,7 +9150,7 @@
         <v>4</v>
       </c>
       <c r="J139" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K139">
         <v>138</v>
@@ -9080,7 +9191,7 @@
         <v>4</v>
       </c>
       <c r="J140" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K140">
         <v>139</v>
@@ -9121,7 +9232,7 @@
         <v>4</v>
       </c>
       <c r="J141" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K141">
         <v>140</v>
@@ -9162,7 +9273,7 @@
         <v>4</v>
       </c>
       <c r="J142" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K142">
         <v>141</v>
@@ -9203,7 +9314,7 @@
         <v>4</v>
       </c>
       <c r="J143" t="s">
-        <v>1022</v>
+        <v>1072</v>
       </c>
       <c r="K143">
         <v>142</v>
@@ -9244,7 +9355,7 @@
         <v>4</v>
       </c>
       <c r="J144" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -9276,7 +9387,7 @@
         <v>4</v>
       </c>
       <c r="J145" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -9308,7 +9419,7 @@
         <v>4</v>
       </c>
       <c r="J146" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -9340,7 +9451,7 @@
         <v>4</v>
       </c>
       <c r="J147" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -9372,7 +9483,7 @@
         <v>4</v>
       </c>
       <c r="J148" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="149" spans="1:10">
@@ -9404,7 +9515,7 @@
         <v>4</v>
       </c>
       <c r="J149" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="150" spans="1:10">
@@ -9436,7 +9547,7 @@
         <v>4</v>
       </c>
       <c r="J150" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -9468,7 +9579,7 @@
         <v>4</v>
       </c>
       <c r="J151" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="152" spans="1:10">
@@ -9500,7 +9611,7 @@
         <v>4</v>
       </c>
       <c r="J152" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="153" spans="1:10">
@@ -9532,7 +9643,7 @@
         <v>4</v>
       </c>
       <c r="J153" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="154" spans="1:10">
@@ -9564,7 +9675,7 @@
         <v>4</v>
       </c>
       <c r="J154" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="155" spans="1:10">
@@ -9596,7 +9707,7 @@
         <v>4</v>
       </c>
       <c r="J155" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="156" spans="1:10">
@@ -9628,7 +9739,7 @@
         <v>4</v>
       </c>
       <c r="J156" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="157" spans="1:10">
@@ -9660,7 +9771,7 @@
         <v>4</v>
       </c>
       <c r="J157" t="s">
-        <v>1023</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="158" spans="1:10">
@@ -9692,7 +9803,7 @@
         <v>4</v>
       </c>
       <c r="J158" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="159" spans="1:10">
@@ -9724,7 +9835,7 @@
         <v>4</v>
       </c>
       <c r="J159" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="160" spans="1:10">
@@ -9756,7 +9867,7 @@
         <v>4</v>
       </c>
       <c r="J160" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="161" spans="1:10">
@@ -9788,7 +9899,7 @@
         <v>4</v>
       </c>
       <c r="J161" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="162" spans="1:10">
@@ -9820,7 +9931,7 @@
         <v>4</v>
       </c>
       <c r="J162" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="163" spans="1:10">
@@ -9852,7 +9963,7 @@
         <v>4</v>
       </c>
       <c r="J163" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="164" spans="1:10">
@@ -9884,7 +9995,7 @@
         <v>4</v>
       </c>
       <c r="J164" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="165" spans="1:10">
@@ -9916,7 +10027,7 @@
         <v>4</v>
       </c>
       <c r="J165" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="166" spans="1:10">
@@ -9948,7 +10059,7 @@
         <v>4</v>
       </c>
       <c r="J166" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="167" spans="1:10">
@@ -9980,7 +10091,7 @@
         <v>4</v>
       </c>
       <c r="J167" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="168" spans="1:10">
@@ -10012,7 +10123,7 @@
         <v>4</v>
       </c>
       <c r="J168" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="169" spans="1:10">
@@ -10044,10 +10155,13 @@
         <v>4</v>
       </c>
       <c r="J169" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="170" spans="1:10">
+      <c r="A170">
+        <v>169</v>
+      </c>
       <c r="B170">
         <v>168</v>
       </c>
@@ -10073,10 +10187,13 @@
         <v>4</v>
       </c>
       <c r="J170" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="171" spans="1:10">
+      <c r="A171">
+        <v>170</v>
+      </c>
       <c r="B171">
         <v>169</v>
       </c>
@@ -10102,356 +10219,1253 @@
         <v>4</v>
       </c>
       <c r="J171" t="s">
-        <v>1024</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="172" spans="1:10">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
       <c r="D172">
         <v>168</v>
       </c>
       <c r="G172" t="s">
         <v>170</v>
       </c>
+      <c r="H172" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I172" s="1">
+        <v>1</v>
+      </c>
+      <c r="J172" t="s">
+        <v>1022</v>
+      </c>
     </row>
     <row r="173" spans="1:10">
+      <c r="C173">
+        <v>2</v>
+      </c>
       <c r="D173">
         <v>169</v>
       </c>
       <c r="G173" t="s">
         <v>171</v>
       </c>
+      <c r="H173" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I173" s="1">
+        <v>1</v>
+      </c>
+      <c r="J173" t="s">
+        <v>1022</v>
+      </c>
     </row>
     <row r="174" spans="1:10">
+      <c r="C174">
+        <v>3</v>
+      </c>
+      <c r="D174">
+        <v>170</v>
+      </c>
       <c r="G174" t="s">
         <v>172</v>
       </c>
+      <c r="H174" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I174" s="1">
+        <v>1</v>
+      </c>
+      <c r="J174" t="s">
+        <v>1022</v>
+      </c>
     </row>
     <row r="175" spans="1:10">
+      <c r="C175">
+        <v>4</v>
+      </c>
+      <c r="D175">
+        <v>171</v>
+      </c>
       <c r="G175" t="s">
         <v>173</v>
       </c>
+      <c r="H175" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I175" s="1">
+        <v>1</v>
+      </c>
+      <c r="J175" t="s">
+        <v>1022</v>
+      </c>
     </row>
     <row r="176" spans="1:10">
+      <c r="C176">
+        <v>5</v>
+      </c>
+      <c r="D176">
+        <v>172</v>
+      </c>
       <c r="G176" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="7:7">
+      <c r="H176" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I176" s="1">
+        <v>1</v>
+      </c>
+      <c r="J176" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="177" spans="3:10">
+      <c r="C177">
+        <v>6</v>
+      </c>
+      <c r="D177">
+        <v>173</v>
+      </c>
       <c r="G177" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="7:7">
+      <c r="H177" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I177" s="1">
+        <v>1</v>
+      </c>
+      <c r="J177" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="178" spans="3:10">
+      <c r="C178">
+        <v>7</v>
+      </c>
+      <c r="D178">
+        <v>174</v>
+      </c>
       <c r="G178" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="7:7">
+      <c r="H178" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I178" s="1">
+        <v>1</v>
+      </c>
+      <c r="J178" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="179" spans="3:10">
+      <c r="C179">
+        <v>8</v>
+      </c>
+      <c r="D179">
+        <v>175</v>
+      </c>
       <c r="G179" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="7:7">
+      <c r="H179" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I179" s="1">
+        <v>1</v>
+      </c>
+      <c r="J179" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="180" spans="3:10">
+      <c r="C180">
+        <v>9</v>
+      </c>
+      <c r="D180">
+        <v>176</v>
+      </c>
       <c r="G180" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="7:7">
+      <c r="H180" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I180" s="1">
+        <v>1</v>
+      </c>
+      <c r="J180" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="181" spans="3:10">
+      <c r="C181">
+        <v>10</v>
+      </c>
+      <c r="D181">
+        <v>177</v>
+      </c>
       <c r="G181" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="7:7">
+      <c r="H181" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I181" s="1">
+        <v>1</v>
+      </c>
+      <c r="J181" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="182" spans="3:10">
+      <c r="C182">
+        <v>11</v>
+      </c>
+      <c r="D182">
+        <v>178</v>
+      </c>
       <c r="G182" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="7:7">
+      <c r="H182" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I182" s="1">
+        <v>1</v>
+      </c>
+      <c r="J182" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="183" spans="3:10">
+      <c r="C183">
+        <v>12</v>
+      </c>
+      <c r="D183">
+        <v>179</v>
+      </c>
       <c r="G183" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="7:7">
+      <c r="H183" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I183" s="1">
+        <v>1</v>
+      </c>
+      <c r="J183" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="184" spans="3:10">
+      <c r="C184">
+        <v>13</v>
+      </c>
+      <c r="D184">
+        <v>180</v>
+      </c>
       <c r="G184" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="7:7">
+      <c r="H184" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I184" s="1">
+        <v>1</v>
+      </c>
+      <c r="J184" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="185" spans="3:10">
+      <c r="C185">
+        <v>14</v>
+      </c>
+      <c r="D185">
+        <v>181</v>
+      </c>
       <c r="G185" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="7:7">
+      <c r="H185" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I185" s="1">
+        <v>1</v>
+      </c>
+      <c r="J185" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="186" spans="3:10">
+      <c r="C186">
+        <v>15</v>
+      </c>
+      <c r="D186">
+        <v>182</v>
+      </c>
       <c r="G186" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="187" spans="7:7">
+      <c r="H186" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I186" s="1">
+        <v>1</v>
+      </c>
+      <c r="J186" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="187" spans="3:10">
+      <c r="C187">
+        <v>16</v>
+      </c>
+      <c r="D187">
+        <v>183</v>
+      </c>
       <c r="G187" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="188" spans="7:7">
+      <c r="H187" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I187" s="1">
+        <v>1</v>
+      </c>
+      <c r="J187" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="188" spans="3:10">
+      <c r="C188">
+        <v>17</v>
+      </c>
+      <c r="D188">
+        <v>184</v>
+      </c>
       <c r="G188" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="7:7">
+      <c r="H188" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I188" s="1">
+        <v>1</v>
+      </c>
+      <c r="J188" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="189" spans="3:10">
+      <c r="C189">
+        <v>18</v>
+      </c>
+      <c r="D189">
+        <v>185</v>
+      </c>
       <c r="G189" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="7:7">
+      <c r="H189" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I189" s="1">
+        <v>1</v>
+      </c>
+      <c r="J189" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="190" spans="3:10">
+      <c r="C190">
+        <v>19</v>
+      </c>
+      <c r="D190">
+        <v>186</v>
+      </c>
       <c r="G190" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="7:7">
+      <c r="H190" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I190" s="1">
+        <v>1</v>
+      </c>
+      <c r="J190" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="191" spans="3:10">
+      <c r="C191">
+        <v>20</v>
+      </c>
+      <c r="D191">
+        <v>187</v>
+      </c>
       <c r="G191" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="7:7">
+      <c r="H191" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I191" s="1">
+        <v>1</v>
+      </c>
+      <c r="J191" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="192" spans="3:10">
+      <c r="C192">
+        <v>21</v>
+      </c>
+      <c r="D192">
+        <v>188</v>
+      </c>
       <c r="G192" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="193" spans="7:7">
+      <c r="H192" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I192" s="1">
+        <v>1</v>
+      </c>
+      <c r="J192" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="193" spans="3:10">
+      <c r="C193">
+        <v>22</v>
+      </c>
+      <c r="D193">
+        <v>189</v>
+      </c>
       <c r="G193" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="194" spans="7:7">
+      <c r="H193" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I193" s="1">
+        <v>1</v>
+      </c>
+      <c r="J193" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="194" spans="3:10">
+      <c r="C194">
+        <v>23</v>
+      </c>
+      <c r="D194">
+        <v>190</v>
+      </c>
       <c r="G194" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="195" spans="7:7">
+      <c r="H194" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I194" s="1">
+        <v>1</v>
+      </c>
+      <c r="J194" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="195" spans="3:10">
+      <c r="C195">
+        <v>24</v>
+      </c>
+      <c r="D195">
+        <v>191</v>
+      </c>
       <c r="G195" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="196" spans="7:7">
+      <c r="H195" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I195" s="1">
+        <v>1</v>
+      </c>
+      <c r="J195" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="196" spans="3:10">
+      <c r="C196">
+        <v>25</v>
+      </c>
+      <c r="D196">
+        <v>192</v>
+      </c>
       <c r="G196" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="197" spans="7:7">
+      <c r="H196" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I196" s="1">
+        <v>1</v>
+      </c>
+      <c r="J196" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="197" spans="3:10">
+      <c r="C197">
+        <v>26</v>
+      </c>
+      <c r="D197">
+        <v>193</v>
+      </c>
       <c r="G197" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="198" spans="7:7">
+      <c r="H197" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I197" s="1">
+        <v>1</v>
+      </c>
+      <c r="J197" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="198" spans="3:10">
+      <c r="C198">
+        <v>27</v>
+      </c>
+      <c r="D198">
+        <v>194</v>
+      </c>
       <c r="G198" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="199" spans="7:7">
+      <c r="H198" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I198" s="1">
+        <v>1</v>
+      </c>
+      <c r="J198" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="199" spans="3:10">
+      <c r="C199">
+        <v>28</v>
+      </c>
+      <c r="D199">
+        <v>195</v>
+      </c>
       <c r="G199" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="200" spans="7:7">
+      <c r="H199" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I199" s="1">
+        <v>1</v>
+      </c>
+      <c r="J199" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="200" spans="3:10">
+      <c r="C200">
+        <v>29</v>
+      </c>
+      <c r="D200">
+        <v>196</v>
+      </c>
       <c r="G200" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="201" spans="7:7">
+      <c r="H200" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I200" s="1">
+        <v>1</v>
+      </c>
+      <c r="J200" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="201" spans="3:10">
+      <c r="C201">
+        <v>30</v>
+      </c>
+      <c r="D201">
+        <v>197</v>
+      </c>
       <c r="G201" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="202" spans="7:7">
+      <c r="H201" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I201" s="1">
+        <v>1</v>
+      </c>
+      <c r="J201" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="202" spans="3:10">
+      <c r="C202">
+        <v>31</v>
+      </c>
+      <c r="D202">
+        <v>198</v>
+      </c>
       <c r="G202" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="203" spans="7:7">
+      <c r="H202" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I202" s="1">
+        <v>2</v>
+      </c>
+      <c r="J202" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="203" spans="3:10">
+      <c r="C203">
+        <v>32</v>
+      </c>
+      <c r="D203">
+        <v>199</v>
+      </c>
       <c r="G203" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="204" spans="7:7">
+      <c r="H203" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I203" s="1">
+        <v>2</v>
+      </c>
+      <c r="J203" s="7" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="204" spans="3:10">
+      <c r="C204">
+        <v>33</v>
+      </c>
+      <c r="D204">
+        <v>200</v>
+      </c>
       <c r="G204" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="205" spans="7:7">
+      <c r="H204" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I204" s="1">
+        <v>2</v>
+      </c>
+      <c r="J204" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="205" spans="3:10">
+      <c r="C205">
+        <v>34</v>
+      </c>
+      <c r="D205">
+        <v>201</v>
+      </c>
       <c r="G205" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="206" spans="7:7">
+      <c r="H205" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I205" s="1">
+        <v>2</v>
+      </c>
+      <c r="J205" s="7" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="206" spans="3:10">
+      <c r="C206">
+        <v>35</v>
+      </c>
+      <c r="D206">
+        <v>202</v>
+      </c>
       <c r="G206" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="207" spans="7:7">
+      <c r="H206" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I206" s="1">
+        <v>2</v>
+      </c>
+      <c r="J206" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="207" spans="3:10">
+      <c r="C207">
+        <v>36</v>
+      </c>
+      <c r="D207">
+        <v>203</v>
+      </c>
       <c r="G207" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="208" spans="7:7">
+      <c r="H207" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I207" s="1">
+        <v>2</v>
+      </c>
+      <c r="J207" s="7" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="208" spans="3:10">
+      <c r="C208">
+        <v>37</v>
+      </c>
+      <c r="D208">
+        <v>204</v>
+      </c>
       <c r="G208" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="209" spans="7:7">
+      <c r="H208" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I208" s="1">
+        <v>2</v>
+      </c>
+      <c r="J208" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="209" spans="3:10">
+      <c r="C209">
+        <v>38</v>
+      </c>
+      <c r="D209">
+        <v>205</v>
+      </c>
       <c r="G209" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="210" spans="7:7">
+      <c r="H209" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I209" s="1">
+        <v>2</v>
+      </c>
+      <c r="J209" s="7" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="210" spans="3:10">
+      <c r="C210">
+        <v>39</v>
+      </c>
+      <c r="D210">
+        <v>206</v>
+      </c>
       <c r="G210" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="211" spans="7:7">
+      <c r="H210" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I210" s="1">
+        <v>2</v>
+      </c>
+      <c r="J210" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="211" spans="3:10">
+      <c r="C211">
+        <v>40</v>
+      </c>
+      <c r="D211">
+        <v>207</v>
+      </c>
       <c r="G211" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="212" spans="7:7">
+      <c r="H211" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I211" s="1">
+        <v>2</v>
+      </c>
+      <c r="J211" s="7" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="212" spans="3:10">
+      <c r="C212">
+        <v>41</v>
+      </c>
+      <c r="D212">
+        <v>208</v>
+      </c>
       <c r="G212" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="213" spans="7:7">
+      <c r="H212" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I212" s="1">
+        <v>2</v>
+      </c>
+      <c r="J212" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="213" spans="3:10">
+      <c r="C213">
+        <v>42</v>
+      </c>
+      <c r="D213">
+        <v>209</v>
+      </c>
       <c r="G213" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="214" spans="7:7">
+      <c r="H213" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I213" s="1">
+        <v>2</v>
+      </c>
+      <c r="J213" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="214" spans="3:10">
+      <c r="C214">
+        <v>43</v>
+      </c>
+      <c r="D214">
+        <v>210</v>
+      </c>
       <c r="G214" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="215" spans="7:7">
+      <c r="H214" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I214" s="1">
+        <v>2</v>
+      </c>
+      <c r="J214" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="215" spans="3:10">
+      <c r="C215">
+        <v>44</v>
+      </c>
+      <c r="D215">
+        <v>211</v>
+      </c>
       <c r="G215" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="216" spans="7:7">
+      <c r="H215" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I215" s="1">
+        <v>2</v>
+      </c>
+      <c r="J215" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="216" spans="3:10">
+      <c r="C216">
+        <v>45</v>
+      </c>
+      <c r="D216">
+        <v>212</v>
+      </c>
       <c r="G216" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="217" spans="7:7">
+      <c r="H216" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I216" s="1">
+        <v>2</v>
+      </c>
+      <c r="J216" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="217" spans="3:10">
+      <c r="C217">
+        <v>46</v>
+      </c>
+      <c r="D217">
+        <v>213</v>
+      </c>
       <c r="G217" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="218" spans="7:7">
+      <c r="H217" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I217" s="1">
+        <v>2</v>
+      </c>
+      <c r="J217" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="218" spans="3:10">
+      <c r="C218">
+        <v>47</v>
+      </c>
+      <c r="D218">
+        <v>214</v>
+      </c>
       <c r="G218" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="219" spans="7:7">
+      <c r="H218" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I218" s="1">
+        <v>2</v>
+      </c>
+      <c r="J218" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="219" spans="3:10">
+      <c r="C219">
+        <v>48</v>
+      </c>
+      <c r="D219">
+        <v>215</v>
+      </c>
       <c r="G219" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="220" spans="7:7">
+      <c r="H219" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I219" s="1">
+        <v>2</v>
+      </c>
+      <c r="J219" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="220" spans="3:10">
+      <c r="C220">
+        <v>49</v>
+      </c>
+      <c r="D220">
+        <v>216</v>
+      </c>
       <c r="G220" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="221" spans="7:7">
+      <c r="H220" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I220" s="1">
+        <v>2</v>
+      </c>
+      <c r="J220" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="221" spans="3:10">
+      <c r="C221">
+        <v>50</v>
+      </c>
+      <c r="D221">
+        <v>217</v>
+      </c>
       <c r="G221" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="222" spans="7:7">
+      <c r="H221" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I221" s="1">
+        <v>2</v>
+      </c>
+      <c r="J221" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="222" spans="3:10">
+      <c r="C222">
+        <v>51</v>
+      </c>
+      <c r="D222">
+        <v>218</v>
+      </c>
       <c r="G222" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="223" spans="7:7">
+      <c r="H222" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I222" s="1">
+        <v>2</v>
+      </c>
+      <c r="J222" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="223" spans="3:10">
+      <c r="C223">
+        <v>52</v>
+      </c>
+      <c r="D223">
+        <v>219</v>
+      </c>
       <c r="G223" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="224" spans="7:7">
+      <c r="H223" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I223" s="1">
+        <v>2</v>
+      </c>
+      <c r="J223" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="224" spans="3:10">
+      <c r="C224">
+        <v>53</v>
+      </c>
+      <c r="D224">
+        <v>220</v>
+      </c>
       <c r="G224" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="225" spans="7:7">
+      <c r="H224" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I224" s="1">
+        <v>2</v>
+      </c>
+      <c r="J224" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="225" spans="3:10">
+      <c r="C225">
+        <v>54</v>
+      </c>
+      <c r="D225">
+        <v>221</v>
+      </c>
       <c r="G225" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="226" spans="7:7">
+      <c r="H225" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I225" s="1">
+        <v>2</v>
+      </c>
+      <c r="J225" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="226" spans="3:10">
+      <c r="C226">
+        <v>55</v>
+      </c>
+      <c r="D226">
+        <v>222</v>
+      </c>
       <c r="G226" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="227" spans="7:7">
+      <c r="H226" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I226" s="1">
+        <v>2</v>
+      </c>
+      <c r="J226" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="227" spans="3:10">
+      <c r="C227">
+        <v>56</v>
+      </c>
+      <c r="D227">
+        <v>223</v>
+      </c>
       <c r="G227" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="228" spans="7:7">
+      <c r="H227" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I227" s="1">
+        <v>2</v>
+      </c>
+      <c r="J227" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="228" spans="3:10">
+      <c r="C228">
+        <v>57</v>
+      </c>
+      <c r="D228">
+        <v>224</v>
+      </c>
       <c r="G228" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="229" spans="7:7">
+      <c r="H228" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I228" s="1">
+        <v>2</v>
+      </c>
+      <c r="J228" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="229" spans="3:10">
+      <c r="C229">
+        <v>58</v>
+      </c>
+      <c r="D229">
+        <v>225</v>
+      </c>
       <c r="G229" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="230" spans="7:7">
+      <c r="H229" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I229" s="1">
+        <v>2</v>
+      </c>
+      <c r="J229" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="230" spans="3:10">
+      <c r="C230">
+        <v>59</v>
+      </c>
+      <c r="D230">
+        <v>226</v>
+      </c>
       <c r="G230" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="231" spans="7:7">
+      <c r="H230" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I230" s="1">
+        <v>2</v>
+      </c>
+      <c r="J230" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="231" spans="3:10">
+      <c r="C231">
+        <v>60</v>
+      </c>
+      <c r="D231">
+        <v>227</v>
+      </c>
       <c r="G231" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="232" spans="7:7">
+      <c r="H231" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I231" s="1">
+        <v>2</v>
+      </c>
+      <c r="J231" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="232" spans="3:10">
       <c r="G232" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="233" spans="7:7">
+    <row r="233" spans="3:10">
       <c r="G233" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="234" spans="7:7">
+    <row r="234" spans="3:10">
       <c r="G234" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="235" spans="7:7">
+    <row r="235" spans="3:10">
       <c r="G235" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="7:7">
+    <row r="236" spans="3:10">
       <c r="G236" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="237" spans="7:7">
+    <row r="237" spans="3:10">
       <c r="G237" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="7:7">
+    <row r="238" spans="3:10">
       <c r="G238" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="7:7">
+    <row r="239" spans="3:10">
       <c r="G239" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="240" spans="7:7">
+    <row r="240" spans="3:10">
       <c r="G240" t="s">
         <v>238</v>
       </c>

</xml_diff>